<commit_message>
code cleanup + add Details class
</commit_message>
<xml_diff>
--- a/Bestelbon.xlsx
+++ b/Bestelbon.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ugentbe-my.sharepoint.com/personal/seppe_vanheulenberghe_ugent_be/Documents/Seppe_2/VT/Snuisters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="8_{BD5CFCD5-8A60-4B84-A229-1BFF477BB48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AD3893D-8033-44B6-BBC1-5C255E8BBB1B}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{BD5CFCD5-8A60-4B84-A229-1BFF477BB48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47710AF5-79A4-4ED7-839A-3AD7E4BF7008}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9F78E8C9-A10A-40EE-A517-0797644B780E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9F78E8C9-A10A-40EE-A517-0797644B780E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Order" sheetId="1" r:id="rId1"/>
+    <sheet name="Details" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Artikel</t>
   </si>
@@ -76,6 +77,12 @@
   </si>
   <si>
     <t>armbanden</t>
+  </si>
+  <si>
+    <t>Ontvanger</t>
+  </si>
+  <si>
+    <t>Template</t>
   </si>
 </sst>
 </file>
@@ -450,9 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED2D40F-DBB6-4748-8CE6-CD83D8EC73E8}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -611,4 +616,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB5AA66-A25E-4A7A-A513-4DF9A51C948D}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add magic method __len__
</commit_message>
<xml_diff>
--- a/Bestelbon.xlsx
+++ b/Bestelbon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ugentbe-my.sharepoint.com/personal/seppe_vanheulenberghe_ugent_be/Documents/Seppe_2/VT/Snuisters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="8_{BD5CFCD5-8A60-4B84-A229-1BFF477BB48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4FE5075-5213-4F86-95F9-4690BE176CF9}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="8_{BD5CFCD5-8A60-4B84-A229-1BFF477BB48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76FDA10E-151D-47A2-A722-917274B83B4F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9F78E8C9-A10A-40EE-A517-0797644B780E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9F78E8C9-A10A-40EE-A517-0797644B780E}"/>
   </bookViews>
   <sheets>
     <sheet name="Order" sheetId="1" r:id="rId1"/>
@@ -88,10 +88,10 @@
     <t>Documentnaam</t>
   </si>
   <si>
-    <t>Isabel</t>
-  </si>
-  <si>
-    <t>BESTELBON_ISABEL</t>
+    <t>Snuisters</t>
+  </si>
+  <si>
+    <t>BESTELBON_SNUISTERS</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED2D40F-DBB6-4748-8CE6-CD83D8EC73E8}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB5AA66-A25E-4A7A-A513-4DF9A51C948D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
adding necessary features for new handlers
</commit_message>
<xml_diff>
--- a/Bestelbon.xlsx
+++ b/Bestelbon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ugentbe-my.sharepoint.com/personal/seppe_vanheulenberghe_ugent_be/Documents/Seppe_2/VT/Snuisters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="8_{BD5CFCD5-8A60-4B84-A229-1BFF477BB48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10EB5305-3D5E-486E-9F2F-61DC2CA7E649}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="8_{BD5CFCD5-8A60-4B84-A229-1BFF477BB48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F362B8D8-BEE3-4C80-8286-D30A8DA394D8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9F78E8C9-A10A-40EE-A517-0797644B780E}"/>
   </bookViews>
@@ -466,7 +466,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -726,7 +726,7 @@
         <v>2.5</v>
       </c>
       <c r="D14" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
fixing problems with invoice
</commit_message>
<xml_diff>
--- a/Bestelbon.xlsx
+++ b/Bestelbon.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ugentbe-my.sharepoint.com/personal/seppe_vanheulenberghe_ugent_be/Documents/Seppe_2/VT/Snuisters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="8_{BD5CFCD5-8A60-4B84-A229-1BFF477BB48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10EB5305-3D5E-486E-9F2F-61DC2CA7E649}"/>
+  <xr:revisionPtr revIDLastSave="323" documentId="8_{BD5CFCD5-8A60-4B84-A229-1BFF477BB48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D975E84E-A0CB-4C28-8B3B-C9E3C8E54039}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9F78E8C9-A10A-40EE-A517-0797644B780E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Artikel</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Winter Sparkle Fine</t>
+  </si>
+  <si>
+    <t>big hoops</t>
   </si>
 </sst>
 </file>
@@ -463,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED2D40F-DBB6-4748-8CE6-CD83D8EC73E8}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -512,9 +515,12 @@
       <c r="D2" s="3">
         <v>5</v>
       </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
       <c r="F2" s="1">
         <f>(B2-C2)*E2</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -530,9 +536,12 @@
       <c r="D3" s="3">
         <v>5</v>
       </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F14" si="0">(B3-C3)*E3</f>
-        <v>0</v>
+        <f t="shared" ref="F3:F15" si="0">(B3-C3)*E3</f>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -548,9 +557,12 @@
       <c r="D4" s="3">
         <v>2</v>
       </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -566,9 +578,12 @@
       <c r="D5" s="3">
         <v>2</v>
       </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>157.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -584,9 +599,12 @@
       <c r="D6" s="3">
         <v>3</v>
       </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -602,9 +620,12 @@
       <c r="D7" s="3">
         <v>4</v>
       </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -620,9 +641,12 @@
       <c r="D8" s="3">
         <v>8</v>
       </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -638,9 +662,12 @@
       <c r="D9" s="3">
         <v>10</v>
       </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -656,9 +683,12 @@
       <c r="D10" s="3">
         <v>1</v>
       </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -674,9 +704,12 @@
       <c r="D11" s="3">
         <v>1</v>
       </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -692,9 +725,12 @@
       <c r="D12" s="3">
         <v>2</v>
       </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -710,9 +746,12 @@
       <c r="D13" s="3">
         <v>1</v>
       </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -728,9 +767,33 @@
       <c r="D14" s="3">
         <v>2</v>
       </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>28.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>